<commit_message>
Fixed bug when determining number of columns/rows on blank sheets
Excel stores information in each worksheet about what part of the sheet is "used". We use this to determine the number of rows or columns in a spreadsheet. When the sheet is empty, though, Excel indicates the "dimension" as A1 (not as a full reference with a colon). So first, we need to account for this when calculating the 'used_area'. Excel also uses 'A1', though, when there is only a value in the cell A1. This commit checks for both of those scenarios and sets the number of rows/columns correctly depending on whether there is data or not.
</commit_message>
<xml_diff>
--- a/tests/Book1.xlsx
+++ b/tests/Book1.xlsx
@@ -5,16 +5,18 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kryan\Lib\dsak\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kryan\Lib\sxl\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7285"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7290"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913" calcMode="manual" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -133,10 +135,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="DateLong" xfId="2"/>
@@ -427,12 +429,12 @@
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.75" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="9.09765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
@@ -505,7 +507,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2">
         <f xml:space="preserve"> R1 + 1</f>
         <v>19</v>
@@ -579,9 +581,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3">
-        <f t="shared" ref="A3:A46" si="1" xml:space="preserve"> R2 + 1</f>
+        <f t="shared" ref="A3:A5" si="1" xml:space="preserve"> R2 + 1</f>
         <v>37</v>
       </c>
       <c r="B3">
@@ -653,7 +655,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" si="1"/>
         <v>55</v>
@@ -727,7 +729,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" si="1"/>
         <v>73</v>
@@ -801,7 +803,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>91</v>
       </c>
@@ -857,7 +859,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>109</v>
       </c>
@@ -914,7 +916,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>127</v>
       </c>
@@ -970,7 +972,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>145</v>
       </c>
@@ -1026,7 +1028,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>163</v>
       </c>
@@ -1082,7 +1084,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>181</v>
       </c>
@@ -1138,7 +1140,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>199</v>
       </c>
@@ -1194,7 +1196,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>217</v>
       </c>
@@ -1250,7 +1252,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>235</v>
       </c>
@@ -1306,7 +1308,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>253</v>
       </c>
@@ -1362,7 +1364,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>271</v>
       </c>
@@ -1384,10 +1386,10 @@
       <c r="G16">
         <v>277</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="H16" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="I16" s="5"/>
+      <c r="I16" s="6"/>
       <c r="J16">
         <v>280</v>
       </c>
@@ -1416,7 +1418,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>289</v>
       </c>
@@ -1472,7 +1474,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>307</v>
       </c>
@@ -1528,7 +1530,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>325</v>
       </c>
@@ -1584,7 +1586,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>343</v>
       </c>
@@ -1640,7 +1642,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>361</v>
       </c>
@@ -1697,7 +1699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>379</v>
       </c>
@@ -1753,7 +1755,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="12" x14ac:dyDescent="0.6">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>397</v>
       </c>
@@ -1809,7 +1811,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>415</v>
       </c>
@@ -1865,7 +1867,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>433</v>
       </c>
@@ -1921,7 +1923,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>451</v>
       </c>
@@ -1977,7 +1979,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>469</v>
       </c>
@@ -2031,7 +2033,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>487</v>
       </c>
@@ -2087,7 +2089,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>505</v>
       </c>
@@ -2143,7 +2145,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>523</v>
       </c>
@@ -2199,7 +2201,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>541</v>
       </c>
@@ -2255,7 +2257,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>559</v>
       </c>
@@ -2271,7 +2273,7 @@
       <c r="E32">
         <v>563</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="F32" s="5" t="s">
         <v>3</v>
       </c>
       <c r="G32">
@@ -2311,7 +2313,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>577</v>
       </c>
@@ -2367,7 +2369,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>595</v>
       </c>
@@ -2423,7 +2425,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>613</v>
       </c>
@@ -2479,7 +2481,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>631</v>
       </c>
@@ -2535,7 +2537,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>649</v>
       </c>
@@ -2591,7 +2593,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>667</v>
       </c>
@@ -2647,7 +2649,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>685</v>
       </c>
@@ -2703,7 +2705,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>703</v>
       </c>
@@ -2759,7 +2761,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>721</v>
       </c>
@@ -2815,7 +2817,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>739</v>
       </c>
@@ -2871,7 +2873,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>757</v>
       </c>
@@ -2927,7 +2929,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>775</v>
       </c>
@@ -2983,7 +2985,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>793</v>
       </c>
@@ -3039,7 +3041,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>811</v>
       </c>
@@ -3102,4 +3104,34 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding new tests to validate time extraction
</commit_message>
<xml_diff>
--- a/tests/Book1.xlsx
+++ b/tests/Book1.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kryan\Lib\sxl\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\lib\python\sxl\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7290"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12000" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Time" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913" calcMode="manual" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -127,7 +128,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
@@ -139,6 +140,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="DateLong" xfId="2"/>
@@ -425,7 +428,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -3120,6 +3123,37 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="7">
+        <v>0.77083333333333337</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
+        <v>0.27083333333333331</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="8">
+        <v>0.60416666666666663</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>